<commit_message>
added pH values to excel file
</commit_message>
<xml_diff>
--- a/excel_filenames_variables.xlsx
+++ b/excel_filenames_variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddharthrath/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddharthrath/Documents/homework_winter_18/direct18project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05642512-864C-6C40-974A-6258A6EB1BAE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705769E2-164F-474E-B3CB-A3D27F3257F5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{47D3C2A5-D602-CC45-89F7-5EDFA5A986E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{47D3C2A5-D602-CC45-89F7-5EDFA5A986E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1277,7 +1277,7 @@
   <dimension ref="A1:H246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,6 +1326,9 @@
       <c r="D2" t="s">
         <v>266</v>
       </c>
+      <c r="E2">
+        <v>6.4</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1346,6 +1349,9 @@
       <c r="D3" t="s">
         <v>266</v>
       </c>
+      <c r="E3">
+        <v>6.4</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1366,6 +1372,9 @@
       <c r="D4" t="s">
         <v>266</v>
       </c>
+      <c r="E4">
+        <v>6.4</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1386,6 +1395,9 @@
       <c r="D5" t="s">
         <v>266</v>
       </c>
+      <c r="E5">
+        <v>6.4</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1406,6 +1418,9 @@
       <c r="D6" t="s">
         <v>266</v>
       </c>
+      <c r="E6">
+        <v>6.4</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1426,6 +1441,9 @@
       <c r="D7" t="s">
         <v>266</v>
       </c>
+      <c r="E7">
+        <v>6.4</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1446,6 +1464,9 @@
       <c r="D8" t="s">
         <v>266</v>
       </c>
+      <c r="E8">
+        <v>6.4</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1465,6 +1486,9 @@
       </c>
       <c r="D9" t="s">
         <v>266</v>
+      </c>
+      <c r="E9">
+        <v>6.4</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>20</v>
@@ -1486,6 +1510,9 @@
       <c r="D10" t="s">
         <v>266</v>
       </c>
+      <c r="E10">
+        <v>6.4</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1506,6 +1533,9 @@
       <c r="D11" t="s">
         <v>266</v>
       </c>
+      <c r="E11">
+        <v>6.4</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1526,6 +1556,9 @@
       <c r="D12" t="s">
         <v>266</v>
       </c>
+      <c r="E12">
+        <v>6.4</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1546,6 +1579,9 @@
       <c r="D13" t="s">
         <v>266</v>
       </c>
+      <c r="E13">
+        <v>6.4</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1566,6 +1602,9 @@
       <c r="D14" t="s">
         <v>266</v>
       </c>
+      <c r="E14">
+        <v>6.4</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1586,6 +1625,9 @@
       <c r="D15" t="s">
         <v>266</v>
       </c>
+      <c r="E15">
+        <v>6.4</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1606,6 +1648,9 @@
       <c r="D16" t="s">
         <v>266</v>
       </c>
+      <c r="E16">
+        <v>6.4</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1626,6 +1671,9 @@
       <c r="D17" t="s">
         <v>266</v>
       </c>
+      <c r="E17">
+        <v>6.4</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1646,6 +1694,9 @@
       <c r="D18" t="s">
         <v>266</v>
       </c>
+      <c r="E18">
+        <v>6.4</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1666,6 +1717,9 @@
       <c r="D19" t="s">
         <v>266</v>
       </c>
+      <c r="E19">
+        <v>6.4</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1686,6 +1740,9 @@
       <c r="D20" t="s">
         <v>266</v>
       </c>
+      <c r="E20">
+        <v>6.4</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1706,6 +1763,9 @@
       <c r="D21" t="s">
         <v>266</v>
       </c>
+      <c r="E21">
+        <v>6.4</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1726,6 +1786,9 @@
       <c r="D22" t="s">
         <v>266</v>
       </c>
+      <c r="E22">
+        <v>6.4</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>33</v>
       </c>
@@ -1746,6 +1809,9 @@
       <c r="D23" t="s">
         <v>266</v>
       </c>
+      <c r="E23">
+        <v>6.4</v>
+      </c>
       <c r="F23" s="1" t="s">
         <v>34</v>
       </c>
@@ -1766,6 +1832,9 @@
       <c r="D24" t="s">
         <v>266</v>
       </c>
+      <c r="E24">
+        <v>6.4</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>35</v>
       </c>
@@ -1786,6 +1855,9 @@
       <c r="D25">
         <v>0</v>
       </c>
+      <c r="E25">
+        <v>7</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1806,6 +1878,9 @@
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1826,6 +1901,9 @@
       <c r="D27">
         <v>0</v>
       </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1846,6 +1924,9 @@
       <c r="D28">
         <v>0</v>
       </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1866,6 +1947,9 @@
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>11</v>
       </c>
@@ -1886,6 +1970,9 @@
       <c r="D30">
         <v>0</v>
       </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1906,6 +1993,9 @@
       <c r="D31" t="s">
         <v>266</v>
       </c>
+      <c r="E31">
+        <v>3.5</v>
+      </c>
       <c r="F31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1923,6 +2013,9 @@
       <c r="D32" t="s">
         <v>266</v>
       </c>
+      <c r="E32">
+        <v>3.5</v>
+      </c>
       <c r="F32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1940,6 +2033,9 @@
       <c r="D33">
         <v>0</v>
       </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
       <c r="F33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1957,6 +2053,9 @@
       <c r="D34" t="s">
         <v>266</v>
       </c>
+      <c r="E34">
+        <v>11</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1974,6 +2073,9 @@
       <c r="D35" t="s">
         <v>266</v>
       </c>
+      <c r="E35">
+        <v>11</v>
+      </c>
       <c r="F35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1991,6 +2093,9 @@
       <c r="D36" t="s">
         <v>266</v>
       </c>
+      <c r="E36">
+        <v>6.4</v>
+      </c>
       <c r="F36" s="1" t="s">
         <v>41</v>
       </c>
@@ -2008,6 +2113,9 @@
       <c r="D37" t="s">
         <v>266</v>
       </c>
+      <c r="E37">
+        <v>6.4</v>
+      </c>
       <c r="F37" s="1" t="s">
         <v>42</v>
       </c>
@@ -2025,6 +2133,9 @@
       <c r="D38" t="s">
         <v>266</v>
       </c>
+      <c r="E38">
+        <v>6.4</v>
+      </c>
       <c r="F38" s="1" t="s">
         <v>43</v>
       </c>
@@ -2042,6 +2153,9 @@
       <c r="D39">
         <v>0</v>
       </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>44</v>
       </c>
@@ -2059,6 +2173,9 @@
       <c r="D40">
         <v>0</v>
       </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>45</v>
       </c>
@@ -2076,6 +2193,9 @@
       <c r="D41">
         <v>0</v>
       </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
       <c r="F41" s="1" t="s">
         <v>46</v>
       </c>
@@ -2093,6 +2213,9 @@
       <c r="D42">
         <v>0</v>
       </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
       <c r="F42" s="1" t="s">
         <v>47</v>
       </c>
@@ -2110,6 +2233,9 @@
       <c r="D43">
         <v>0</v>
       </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
       <c r="F43" s="1" t="s">
         <v>48</v>
       </c>
@@ -2127,6 +2253,9 @@
       <c r="D44">
         <v>0</v>
       </c>
+      <c r="E44">
+        <v>7</v>
+      </c>
       <c r="F44" s="1" t="s">
         <v>49</v>
       </c>
@@ -2144,6 +2273,9 @@
       <c r="D45" t="s">
         <v>267</v>
       </c>
+      <c r="E45">
+        <v>6.4</v>
+      </c>
       <c r="F45" s="1" t="s">
         <v>50</v>
       </c>
@@ -2161,6 +2293,9 @@
       <c r="D46" t="s">
         <v>267</v>
       </c>
+      <c r="E46">
+        <v>6.4</v>
+      </c>
       <c r="F46" s="1" t="s">
         <v>51</v>
       </c>
@@ -2178,6 +2313,9 @@
       <c r="D47" t="s">
         <v>267</v>
       </c>
+      <c r="E47">
+        <v>6.4</v>
+      </c>
       <c r="F47" s="1" t="s">
         <v>52</v>
       </c>
@@ -2195,6 +2333,9 @@
       <c r="D48" t="s">
         <v>267</v>
       </c>
+      <c r="E48">
+        <v>6.4</v>
+      </c>
       <c r="F48" s="1" t="s">
         <v>53</v>
       </c>
@@ -2212,6 +2353,9 @@
       <c r="D49" t="s">
         <v>267</v>
       </c>
+      <c r="E49">
+        <v>6.4</v>
+      </c>
       <c r="F49" s="1" t="s">
         <v>54</v>
       </c>
@@ -2229,6 +2373,9 @@
       <c r="D50" t="s">
         <v>267</v>
       </c>
+      <c r="E50">
+        <v>6.4</v>
+      </c>
       <c r="F50" s="1" t="s">
         <v>55</v>
       </c>
@@ -2246,6 +2393,9 @@
       <c r="D51" t="s">
         <v>267</v>
       </c>
+      <c r="E51">
+        <v>6.4</v>
+      </c>
       <c r="F51" s="1" t="s">
         <v>56</v>
       </c>
@@ -2263,6 +2413,9 @@
       <c r="D52" t="s">
         <v>267</v>
       </c>
+      <c r="E52">
+        <v>6.4</v>
+      </c>
       <c r="F52" s="1" t="s">
         <v>57</v>
       </c>
@@ -2280,6 +2433,9 @@
       <c r="D53" t="s">
         <v>267</v>
       </c>
+      <c r="E53">
+        <v>6.4</v>
+      </c>
       <c r="F53" s="1" t="s">
         <v>58</v>
       </c>
@@ -2297,6 +2453,9 @@
       <c r="D54" t="s">
         <v>267</v>
       </c>
+      <c r="E54">
+        <v>6.4</v>
+      </c>
       <c r="F54" s="1" t="s">
         <v>59</v>
       </c>
@@ -2314,6 +2473,9 @@
       <c r="D55" t="s">
         <v>268</v>
       </c>
+      <c r="E55">
+        <v>6.4</v>
+      </c>
       <c r="F55" s="1" t="s">
         <v>60</v>
       </c>
@@ -2331,6 +2493,9 @@
       <c r="D56" t="s">
         <v>268</v>
       </c>
+      <c r="E56">
+        <v>6.4</v>
+      </c>
       <c r="F56" s="1" t="s">
         <v>61</v>
       </c>
@@ -2348,6 +2513,9 @@
       <c r="D57" t="s">
         <v>268</v>
       </c>
+      <c r="E57">
+        <v>6.4</v>
+      </c>
       <c r="F57" s="1" t="s">
         <v>62</v>
       </c>
@@ -2365,6 +2533,9 @@
       <c r="D58" t="s">
         <v>266</v>
       </c>
+      <c r="E58">
+        <v>6.4</v>
+      </c>
       <c r="F58" s="1" t="s">
         <v>63</v>
       </c>
@@ -2382,6 +2553,9 @@
       <c r="D59" t="s">
         <v>266</v>
       </c>
+      <c r="E59">
+        <v>6.4</v>
+      </c>
       <c r="F59" s="1" t="s">
         <v>64</v>
       </c>
@@ -2399,6 +2573,9 @@
       <c r="D60" t="s">
         <v>266</v>
       </c>
+      <c r="E60">
+        <v>6.4</v>
+      </c>
       <c r="F60" s="1" t="s">
         <v>65</v>
       </c>
@@ -2416,6 +2593,9 @@
       <c r="D61" t="s">
         <v>266</v>
       </c>
+      <c r="E61">
+        <v>6.4</v>
+      </c>
       <c r="F61" s="1" t="s">
         <v>66</v>
       </c>
@@ -2433,6 +2613,9 @@
       <c r="D62" t="s">
         <v>266</v>
       </c>
+      <c r="E62">
+        <v>6.4</v>
+      </c>
       <c r="F62" s="1" t="s">
         <v>67</v>
       </c>
@@ -2450,6 +2633,9 @@
       <c r="D63" t="s">
         <v>266</v>
       </c>
+      <c r="E63">
+        <v>6.4</v>
+      </c>
       <c r="F63" s="1" t="s">
         <v>68</v>
       </c>
@@ -2467,6 +2653,9 @@
       <c r="D64">
         <v>0</v>
       </c>
+      <c r="E64">
+        <v>7</v>
+      </c>
       <c r="F64" s="1" t="s">
         <v>69</v>
       </c>
@@ -2484,6 +2673,9 @@
       <c r="D65">
         <v>0</v>
       </c>
+      <c r="E65">
+        <v>7</v>
+      </c>
       <c r="F65" s="1" t="s">
         <v>70</v>
       </c>
@@ -2501,6 +2693,9 @@
       <c r="D66" t="s">
         <v>268</v>
       </c>
+      <c r="E66">
+        <v>6.4</v>
+      </c>
       <c r="F66" s="1" t="s">
         <v>71</v>
       </c>
@@ -2518,6 +2713,9 @@
       <c r="D67" t="s">
         <v>268</v>
       </c>
+      <c r="E67">
+        <v>6.4</v>
+      </c>
       <c r="F67" s="1" t="s">
         <v>72</v>
       </c>
@@ -2535,6 +2733,9 @@
       <c r="D68" t="s">
         <v>268</v>
       </c>
+      <c r="E68">
+        <v>6.4</v>
+      </c>
       <c r="F68" s="1" t="s">
         <v>73</v>
       </c>
@@ -2552,6 +2753,9 @@
       <c r="D69" t="s">
         <v>268</v>
       </c>
+      <c r="E69">
+        <v>6.4</v>
+      </c>
       <c r="F69" s="1" t="s">
         <v>74</v>
       </c>
@@ -2569,6 +2773,9 @@
       <c r="D70" t="s">
         <v>268</v>
       </c>
+      <c r="E70">
+        <v>6.4</v>
+      </c>
       <c r="F70" s="1" t="s">
         <v>75</v>
       </c>
@@ -2586,6 +2793,9 @@
       <c r="D71" t="s">
         <v>266</v>
       </c>
+      <c r="E71">
+        <v>6.4</v>
+      </c>
       <c r="F71" s="1" t="s">
         <v>76</v>
       </c>
@@ -2603,6 +2813,9 @@
       <c r="D72" t="s">
         <v>266</v>
       </c>
+      <c r="E72">
+        <v>6.4</v>
+      </c>
       <c r="F72" s="1" t="s">
         <v>77</v>
       </c>
@@ -2620,6 +2833,9 @@
       <c r="D73" t="s">
         <v>266</v>
       </c>
+      <c r="E73">
+        <v>6.4</v>
+      </c>
       <c r="F73" s="1" t="s">
         <v>78</v>
       </c>
@@ -2637,6 +2853,9 @@
       <c r="D74" t="s">
         <v>266</v>
       </c>
+      <c r="E74">
+        <v>6.4</v>
+      </c>
       <c r="F74" s="1" t="s">
         <v>79</v>
       </c>
@@ -2654,6 +2873,9 @@
       <c r="D75" t="s">
         <v>267</v>
       </c>
+      <c r="E75">
+        <v>6.4</v>
+      </c>
       <c r="F75" s="1" t="s">
         <v>80</v>
       </c>
@@ -2671,6 +2893,9 @@
       <c r="D76" t="s">
         <v>267</v>
       </c>
+      <c r="E76">
+        <v>6.4</v>
+      </c>
       <c r="F76" s="1" t="s">
         <v>81</v>
       </c>
@@ -2688,6 +2913,9 @@
       <c r="D77">
         <v>0</v>
       </c>
+      <c r="E77">
+        <v>7</v>
+      </c>
       <c r="F77" s="1" t="s">
         <v>82</v>
       </c>
@@ -2705,6 +2933,9 @@
       <c r="D78">
         <v>0</v>
       </c>
+      <c r="E78">
+        <v>7</v>
+      </c>
       <c r="F78" s="1" t="s">
         <v>83</v>
       </c>
@@ -2722,6 +2953,9 @@
       <c r="D79">
         <v>0</v>
       </c>
+      <c r="E79">
+        <v>7</v>
+      </c>
       <c r="F79" s="1" t="s">
         <v>84</v>
       </c>
@@ -2739,6 +2973,9 @@
       <c r="D80">
         <v>0</v>
       </c>
+      <c r="E80">
+        <v>7</v>
+      </c>
       <c r="F80" s="1" t="s">
         <v>85</v>
       </c>
@@ -2756,6 +2993,9 @@
       <c r="D81" t="s">
         <v>267</v>
       </c>
+      <c r="E81">
+        <v>6.4</v>
+      </c>
       <c r="F81" s="1" t="s">
         <v>86</v>
       </c>
@@ -2773,6 +3013,9 @@
       <c r="D82" t="s">
         <v>267</v>
       </c>
+      <c r="E82">
+        <v>6.4</v>
+      </c>
       <c r="F82" s="1" t="s">
         <v>87</v>
       </c>
@@ -2790,6 +3033,9 @@
       <c r="D83" t="s">
         <v>266</v>
       </c>
+      <c r="E83">
+        <v>6.4</v>
+      </c>
       <c r="F83" s="1" t="s">
         <v>88</v>
       </c>
@@ -2807,6 +3053,9 @@
       <c r="D84" t="s">
         <v>266</v>
       </c>
+      <c r="E84">
+        <v>6.4</v>
+      </c>
       <c r="F84" s="1" t="s">
         <v>89</v>
       </c>
@@ -2824,6 +3073,9 @@
       <c r="D85" t="s">
         <v>266</v>
       </c>
+      <c r="E85">
+        <v>6.4</v>
+      </c>
       <c r="F85" s="1" t="s">
         <v>90</v>
       </c>
@@ -2841,6 +3093,9 @@
       <c r="D86">
         <v>0</v>
       </c>
+      <c r="E86">
+        <v>7</v>
+      </c>
       <c r="F86" s="1" t="s">
         <v>91</v>
       </c>
@@ -2858,6 +3113,9 @@
       <c r="D87">
         <v>0</v>
       </c>
+      <c r="E87">
+        <v>7</v>
+      </c>
       <c r="F87" s="1" t="s">
         <v>92</v>
       </c>
@@ -2875,6 +3133,9 @@
       <c r="D88" t="s">
         <v>267</v>
       </c>
+      <c r="E88">
+        <v>6.4</v>
+      </c>
       <c r="F88" s="1" t="s">
         <v>93</v>
       </c>
@@ -2892,6 +3153,9 @@
       <c r="D89" t="s">
         <v>267</v>
       </c>
+      <c r="E89">
+        <v>6.4</v>
+      </c>
       <c r="F89" s="1" t="s">
         <v>94</v>
       </c>
@@ -2909,6 +3173,9 @@
       <c r="D90" t="s">
         <v>269</v>
       </c>
+      <c r="E90">
+        <v>6.4</v>
+      </c>
       <c r="F90" s="1" t="s">
         <v>95</v>
       </c>
@@ -2926,6 +3193,9 @@
       <c r="D91" t="s">
         <v>269</v>
       </c>
+      <c r="E91">
+        <v>6.4</v>
+      </c>
       <c r="F91" s="1" t="s">
         <v>96</v>
       </c>
@@ -2943,6 +3213,9 @@
       <c r="D92" t="s">
         <v>270</v>
       </c>
+      <c r="E92">
+        <v>6.4</v>
+      </c>
       <c r="F92" s="1" t="s">
         <v>97</v>
       </c>
@@ -2960,6 +3233,9 @@
       <c r="D93" t="s">
         <v>270</v>
       </c>
+      <c r="E93">
+        <v>6.4</v>
+      </c>
       <c r="F93" s="1" t="s">
         <v>98</v>
       </c>
@@ -2977,6 +3253,9 @@
       <c r="D94" t="s">
         <v>270</v>
       </c>
+      <c r="E94">
+        <v>6.4</v>
+      </c>
       <c r="F94" s="1" t="s">
         <v>99</v>
       </c>
@@ -2994,6 +3273,9 @@
       <c r="D95" t="s">
         <v>267</v>
       </c>
+      <c r="E95">
+        <v>6.4</v>
+      </c>
       <c r="F95" s="1" t="s">
         <v>100</v>
       </c>
@@ -3011,6 +3293,9 @@
       <c r="D96" t="s">
         <v>268</v>
       </c>
+      <c r="E96">
+        <v>6.4</v>
+      </c>
       <c r="F96" s="1" t="s">
         <v>101</v>
       </c>
@@ -3028,6 +3313,9 @@
       <c r="D97" t="s">
         <v>266</v>
       </c>
+      <c r="E97">
+        <v>6.4</v>
+      </c>
       <c r="F97" s="1" t="s">
         <v>102</v>
       </c>
@@ -3045,6 +3333,9 @@
       <c r="D98" t="s">
         <v>266</v>
       </c>
+      <c r="E98">
+        <v>6.4</v>
+      </c>
       <c r="F98" s="1" t="s">
         <v>103</v>
       </c>
@@ -3062,6 +3353,9 @@
       <c r="D99" t="s">
         <v>266</v>
       </c>
+      <c r="E99">
+        <v>6.4</v>
+      </c>
       <c r="F99" s="1" t="s">
         <v>104</v>
       </c>
@@ -3079,6 +3373,9 @@
       <c r="D100" t="s">
         <v>267</v>
       </c>
+      <c r="E100">
+        <v>6.4</v>
+      </c>
       <c r="F100" s="1" t="s">
         <v>105</v>
       </c>
@@ -3096,6 +3393,9 @@
       <c r="D101" t="s">
         <v>268</v>
       </c>
+      <c r="E101">
+        <v>6.4</v>
+      </c>
       <c r="F101" s="1" t="s">
         <v>106</v>
       </c>
@@ -3113,6 +3413,9 @@
       <c r="D102" t="s">
         <v>268</v>
       </c>
+      <c r="E102">
+        <v>6.4</v>
+      </c>
       <c r="F102" s="1" t="s">
         <v>107</v>
       </c>
@@ -3130,6 +3433,9 @@
       <c r="D103" t="s">
         <v>266</v>
       </c>
+      <c r="E103">
+        <v>6.4</v>
+      </c>
       <c r="F103" s="1" t="s">
         <v>108</v>
       </c>
@@ -3147,6 +3453,9 @@
       <c r="D104" t="s">
         <v>266</v>
       </c>
+      <c r="E104">
+        <v>6.4</v>
+      </c>
       <c r="F104" s="1" t="s">
         <v>109</v>
       </c>
@@ -3164,6 +3473,9 @@
       <c r="D105" t="s">
         <v>266</v>
       </c>
+      <c r="E105">
+        <v>6.4</v>
+      </c>
       <c r="F105" s="1" t="s">
         <v>110</v>
       </c>
@@ -3181,6 +3493,9 @@
       <c r="D106" t="s">
         <v>266</v>
       </c>
+      <c r="E106">
+        <v>6.4</v>
+      </c>
       <c r="F106" s="1" t="s">
         <v>111</v>
       </c>
@@ -3198,6 +3513,9 @@
       <c r="D107">
         <v>0</v>
       </c>
+      <c r="E107">
+        <v>7</v>
+      </c>
       <c r="F107" s="1" t="s">
         <v>112</v>
       </c>
@@ -3215,6 +3533,9 @@
       <c r="D108">
         <v>0</v>
       </c>
+      <c r="E108">
+        <v>7</v>
+      </c>
       <c r="F108" s="1" t="s">
         <v>113</v>
       </c>
@@ -3232,6 +3553,9 @@
       <c r="D109">
         <v>0</v>
       </c>
+      <c r="E109">
+        <v>7</v>
+      </c>
       <c r="F109" s="1" t="s">
         <v>114</v>
       </c>
@@ -3249,6 +3573,9 @@
       <c r="D110">
         <v>0</v>
       </c>
+      <c r="E110">
+        <v>7</v>
+      </c>
       <c r="F110" s="1" t="s">
         <v>115</v>
       </c>
@@ -3266,6 +3593,9 @@
       <c r="D111">
         <v>0</v>
       </c>
+      <c r="E111">
+        <v>7</v>
+      </c>
       <c r="F111" s="1" t="s">
         <v>116</v>
       </c>
@@ -3283,6 +3613,9 @@
       <c r="D112">
         <v>0</v>
       </c>
+      <c r="E112">
+        <v>7</v>
+      </c>
       <c r="F112" s="1" t="s">
         <v>117</v>
       </c>
@@ -3300,6 +3633,9 @@
       <c r="D113">
         <v>0</v>
       </c>
+      <c r="E113">
+        <v>7</v>
+      </c>
       <c r="F113" s="1" t="s">
         <v>118</v>
       </c>
@@ -3317,6 +3653,9 @@
       <c r="D114">
         <v>0</v>
       </c>
+      <c r="E114">
+        <v>7</v>
+      </c>
       <c r="F114" s="1" t="s">
         <v>119</v>
       </c>
@@ -3334,6 +3673,9 @@
       <c r="D115" t="s">
         <v>267</v>
       </c>
+      <c r="E115">
+        <v>6.4</v>
+      </c>
       <c r="F115" s="1" t="s">
         <v>120</v>
       </c>
@@ -3351,6 +3693,9 @@
       <c r="D116" t="s">
         <v>267</v>
       </c>
+      <c r="E116">
+        <v>6.4</v>
+      </c>
       <c r="F116" s="1" t="s">
         <v>121</v>
       </c>
@@ -3368,6 +3713,9 @@
       <c r="D117" t="s">
         <v>268</v>
       </c>
+      <c r="E117">
+        <v>6.4</v>
+      </c>
       <c r="F117" s="1" t="s">
         <v>122</v>
       </c>
@@ -3385,6 +3733,9 @@
       <c r="D118" t="s">
         <v>268</v>
       </c>
+      <c r="E118">
+        <v>6.4</v>
+      </c>
       <c r="F118" s="1" t="s">
         <v>123</v>
       </c>
@@ -3402,6 +3753,9 @@
       <c r="D119" t="s">
         <v>268</v>
       </c>
+      <c r="E119">
+        <v>6.4</v>
+      </c>
       <c r="F119" s="1" t="s">
         <v>124</v>
       </c>
@@ -3419,6 +3773,9 @@
       <c r="D120" t="s">
         <v>268</v>
       </c>
+      <c r="E120">
+        <v>6.4</v>
+      </c>
       <c r="F120" s="1" t="s">
         <v>125</v>
       </c>
@@ -3436,6 +3793,9 @@
       <c r="D121" t="s">
         <v>266</v>
       </c>
+      <c r="E121">
+        <v>6.4</v>
+      </c>
       <c r="F121" s="1" t="s">
         <v>126</v>
       </c>
@@ -3453,6 +3813,9 @@
       <c r="D122" t="s">
         <v>266</v>
       </c>
+      <c r="E122">
+        <v>6.4</v>
+      </c>
       <c r="F122" s="1" t="s">
         <v>127</v>
       </c>
@@ -3470,6 +3833,9 @@
       <c r="D123" t="s">
         <v>266</v>
       </c>
+      <c r="E123">
+        <v>6.4</v>
+      </c>
       <c r="F123" s="1" t="s">
         <v>128</v>
       </c>
@@ -3487,6 +3853,9 @@
       <c r="D124" t="s">
         <v>266</v>
       </c>
+      <c r="E124">
+        <v>6.4</v>
+      </c>
       <c r="F124" s="1" t="s">
         <v>129</v>
       </c>
@@ -3504,6 +3873,9 @@
       <c r="D125">
         <v>0</v>
       </c>
+      <c r="E125">
+        <v>7</v>
+      </c>
       <c r="F125" s="1" t="s">
         <v>130</v>
       </c>
@@ -3521,6 +3893,9 @@
       <c r="D126" t="s">
         <v>267</v>
       </c>
+      <c r="E126">
+        <v>6.4</v>
+      </c>
       <c r="F126" s="1" t="s">
         <v>131</v>
       </c>
@@ -3538,6 +3913,9 @@
       <c r="D127" t="s">
         <v>267</v>
       </c>
+      <c r="E127">
+        <v>6.4</v>
+      </c>
       <c r="F127" s="1" t="s">
         <v>132</v>
       </c>
@@ -3555,6 +3933,9 @@
       <c r="D128" t="s">
         <v>268</v>
       </c>
+      <c r="E128">
+        <v>6.4</v>
+      </c>
       <c r="F128" s="1" t="s">
         <v>133</v>
       </c>
@@ -3572,6 +3953,9 @@
       <c r="D129" t="s">
         <v>268</v>
       </c>
+      <c r="E129">
+        <v>6.4</v>
+      </c>
       <c r="F129" s="1" t="s">
         <v>134</v>
       </c>
@@ -3589,6 +3973,9 @@
       <c r="D130" t="s">
         <v>266</v>
       </c>
+      <c r="E130">
+        <v>6.4</v>
+      </c>
       <c r="F130" s="1" t="s">
         <v>135</v>
       </c>
@@ -3606,6 +3993,9 @@
       <c r="D131">
         <v>0</v>
       </c>
+      <c r="E131">
+        <v>7</v>
+      </c>
       <c r="F131" s="1" t="s">
         <v>136</v>
       </c>
@@ -3623,6 +4013,9 @@
       <c r="D132">
         <v>0</v>
       </c>
+      <c r="E132">
+        <v>7</v>
+      </c>
       <c r="F132" s="1" t="s">
         <v>137</v>
       </c>
@@ -3640,6 +4033,9 @@
       <c r="D133">
         <v>0</v>
       </c>
+      <c r="E133">
+        <v>7</v>
+      </c>
       <c r="F133" s="1" t="s">
         <v>138</v>
       </c>
@@ -3657,6 +4053,9 @@
       <c r="D134">
         <v>0</v>
       </c>
+      <c r="E134">
+        <v>7</v>
+      </c>
       <c r="F134" s="1" t="s">
         <v>139</v>
       </c>
@@ -3674,6 +4073,9 @@
       <c r="D135">
         <v>0</v>
       </c>
+      <c r="E135">
+        <v>7</v>
+      </c>
       <c r="F135" s="1" t="s">
         <v>140</v>
       </c>
@@ -3691,6 +4093,9 @@
       <c r="D136">
         <v>0</v>
       </c>
+      <c r="E136">
+        <v>7</v>
+      </c>
       <c r="F136" s="1" t="s">
         <v>141</v>
       </c>
@@ -3708,6 +4113,9 @@
       <c r="D137" t="s">
         <v>267</v>
       </c>
+      <c r="E137">
+        <v>6.4</v>
+      </c>
       <c r="F137" s="1" t="s">
         <v>142</v>
       </c>
@@ -3725,6 +4133,9 @@
       <c r="D138" t="s">
         <v>267</v>
       </c>
+      <c r="E138">
+        <v>6.4</v>
+      </c>
       <c r="F138" s="1" t="s">
         <v>143</v>
       </c>
@@ -3742,6 +4153,9 @@
       <c r="D139" t="s">
         <v>267</v>
       </c>
+      <c r="E139">
+        <v>6.4</v>
+      </c>
       <c r="F139" s="1" t="s">
         <v>144</v>
       </c>
@@ -3759,6 +4173,9 @@
       <c r="D140" t="s">
         <v>267</v>
       </c>
+      <c r="E140">
+        <v>6.4</v>
+      </c>
       <c r="F140" s="1" t="s">
         <v>145</v>
       </c>
@@ -3776,6 +4193,9 @@
       <c r="D141" t="s">
         <v>267</v>
       </c>
+      <c r="E141">
+        <v>6.4</v>
+      </c>
       <c r="F141" s="1" t="s">
         <v>146</v>
       </c>
@@ -3793,6 +4213,9 @@
       <c r="D142" t="s">
         <v>268</v>
       </c>
+      <c r="E142">
+        <v>6.4</v>
+      </c>
       <c r="F142" s="1" t="s">
         <v>147</v>
       </c>
@@ -3810,6 +4233,9 @@
       <c r="D143" t="s">
         <v>268</v>
       </c>
+      <c r="E143">
+        <v>6.4</v>
+      </c>
       <c r="F143" s="1" t="s">
         <v>148</v>
       </c>
@@ -3827,6 +4253,9 @@
       <c r="D144" t="s">
         <v>268</v>
       </c>
+      <c r="E144">
+        <v>6.4</v>
+      </c>
       <c r="F144" s="1" t="s">
         <v>149</v>
       </c>
@@ -3844,6 +4273,9 @@
       <c r="D145" t="s">
         <v>268</v>
       </c>
+      <c r="E145">
+        <v>6.4</v>
+      </c>
       <c r="F145" s="1" t="s">
         <v>150</v>
       </c>
@@ -3861,6 +4293,9 @@
       <c r="D146" t="s">
         <v>268</v>
       </c>
+      <c r="E146">
+        <v>6.4</v>
+      </c>
       <c r="F146" s="1" t="s">
         <v>151</v>
       </c>
@@ -3878,6 +4313,9 @@
       <c r="D147" t="s">
         <v>268</v>
       </c>
+      <c r="E147">
+        <v>6.4</v>
+      </c>
       <c r="F147" s="1" t="s">
         <v>152</v>
       </c>
@@ -3895,6 +4333,9 @@
       <c r="D148" t="s">
         <v>266</v>
       </c>
+      <c r="E148">
+        <v>6.4</v>
+      </c>
       <c r="F148" s="1" t="s">
         <v>153</v>
       </c>
@@ -3912,6 +4353,9 @@
       <c r="D149" t="s">
         <v>266</v>
       </c>
+      <c r="E149">
+        <v>6.4</v>
+      </c>
       <c r="F149" s="1" t="s">
         <v>154</v>
       </c>
@@ -3929,6 +4373,9 @@
       <c r="D150" t="s">
         <v>266</v>
       </c>
+      <c r="E150">
+        <v>6.4</v>
+      </c>
       <c r="F150" s="1" t="s">
         <v>155</v>
       </c>
@@ -3946,6 +4393,9 @@
       <c r="D151" t="s">
         <v>266</v>
       </c>
+      <c r="E151">
+        <v>6.4</v>
+      </c>
       <c r="F151" s="1" t="s">
         <v>156</v>
       </c>
@@ -3963,6 +4413,9 @@
       <c r="D152" t="s">
         <v>266</v>
       </c>
+      <c r="E152">
+        <v>6.4</v>
+      </c>
       <c r="F152" s="1" t="s">
         <v>157</v>
       </c>
@@ -3980,6 +4433,9 @@
       <c r="D153" t="s">
         <v>266</v>
       </c>
+      <c r="E153">
+        <v>6.4</v>
+      </c>
       <c r="F153" s="1" t="s">
         <v>158</v>
       </c>
@@ -3997,6 +4453,9 @@
       <c r="D154" t="s">
         <v>266</v>
       </c>
+      <c r="E154">
+        <v>6.4</v>
+      </c>
       <c r="F154" s="1" t="s">
         <v>159</v>
       </c>
@@ -4014,6 +4473,9 @@
       <c r="D155" t="s">
         <v>266</v>
       </c>
+      <c r="E155">
+        <v>6.4</v>
+      </c>
       <c r="F155" s="1" t="s">
         <v>160</v>
       </c>
@@ -4031,6 +4493,9 @@
       <c r="D156">
         <v>0</v>
       </c>
+      <c r="E156">
+        <v>7</v>
+      </c>
       <c r="F156" s="1" t="s">
         <v>161</v>
       </c>
@@ -4048,6 +4513,9 @@
       <c r="D157">
         <v>0</v>
       </c>
+      <c r="E157">
+        <v>7</v>
+      </c>
       <c r="F157" s="1" t="s">
         <v>162</v>
       </c>
@@ -4065,6 +4533,9 @@
       <c r="D158">
         <v>0</v>
       </c>
+      <c r="E158">
+        <v>7</v>
+      </c>
       <c r="F158" s="1" t="s">
         <v>163</v>
       </c>
@@ -4082,6 +4553,9 @@
       <c r="D159">
         <v>0</v>
       </c>
+      <c r="E159">
+        <v>7</v>
+      </c>
       <c r="F159" s="1" t="s">
         <v>164</v>
       </c>
@@ -4099,6 +4573,9 @@
       <c r="D160">
         <v>0</v>
       </c>
+      <c r="E160">
+        <v>7</v>
+      </c>
       <c r="F160" s="1" t="s">
         <v>165</v>
       </c>
@@ -4116,6 +4593,9 @@
       <c r="D161">
         <v>0</v>
       </c>
+      <c r="E161">
+        <v>7</v>
+      </c>
       <c r="F161" s="1" t="s">
         <v>166</v>
       </c>
@@ -4133,6 +4613,9 @@
       <c r="D162">
         <v>0</v>
       </c>
+      <c r="E162">
+        <v>7</v>
+      </c>
       <c r="F162" s="1" t="s">
         <v>167</v>
       </c>
@@ -4150,6 +4633,9 @@
       <c r="D163">
         <v>0</v>
       </c>
+      <c r="E163">
+        <v>7</v>
+      </c>
       <c r="F163" s="1" t="s">
         <v>168</v>
       </c>
@@ -4167,6 +4653,9 @@
       <c r="D164">
         <v>0</v>
       </c>
+      <c r="E164">
+        <v>7</v>
+      </c>
       <c r="F164" s="1" t="s">
         <v>169</v>
       </c>
@@ -4184,6 +4673,9 @@
       <c r="D165">
         <v>0</v>
       </c>
+      <c r="E165">
+        <v>7</v>
+      </c>
       <c r="F165" s="1" t="s">
         <v>170</v>
       </c>
@@ -4201,6 +4693,9 @@
       <c r="D166" t="s">
         <v>268</v>
       </c>
+      <c r="E166">
+        <v>6.4</v>
+      </c>
       <c r="F166" s="1" t="s">
         <v>171</v>
       </c>
@@ -4218,6 +4713,9 @@
       <c r="D167" t="s">
         <v>268</v>
       </c>
+      <c r="E167">
+        <v>6.4</v>
+      </c>
       <c r="F167" s="1" t="s">
         <v>172</v>
       </c>
@@ -4235,6 +4733,9 @@
       <c r="D168" t="s">
         <v>268</v>
       </c>
+      <c r="E168">
+        <v>6.4</v>
+      </c>
       <c r="F168" s="1" t="s">
         <v>173</v>
       </c>
@@ -4252,6 +4753,9 @@
       <c r="D169" t="s">
         <v>268</v>
       </c>
+      <c r="E169">
+        <v>6.4</v>
+      </c>
       <c r="F169" s="1" t="s">
         <v>174</v>
       </c>
@@ -4269,6 +4773,9 @@
       <c r="D170" t="s">
         <v>268</v>
       </c>
+      <c r="E170">
+        <v>6.4</v>
+      </c>
       <c r="F170" s="1" t="s">
         <v>175</v>
       </c>
@@ -4286,6 +4793,9 @@
       <c r="D171" t="s">
         <v>268</v>
       </c>
+      <c r="E171">
+        <v>6.4</v>
+      </c>
       <c r="F171" s="1" t="s">
         <v>176</v>
       </c>
@@ -4303,6 +4813,9 @@
       <c r="D172" t="s">
         <v>268</v>
       </c>
+      <c r="E172">
+        <v>6.4</v>
+      </c>
       <c r="F172" s="1" t="s">
         <v>177</v>
       </c>
@@ -4320,6 +4833,9 @@
       <c r="D173" t="s">
         <v>266</v>
       </c>
+      <c r="E173">
+        <v>6.4</v>
+      </c>
       <c r="F173" s="1" t="s">
         <v>178</v>
       </c>
@@ -4337,6 +4853,9 @@
       <c r="D174" t="s">
         <v>266</v>
       </c>
+      <c r="E174">
+        <v>6.4</v>
+      </c>
       <c r="F174" s="1" t="s">
         <v>179</v>
       </c>
@@ -4354,6 +4873,9 @@
       <c r="D175" t="s">
         <v>266</v>
       </c>
+      <c r="E175">
+        <v>6.4</v>
+      </c>
       <c r="F175" s="1" t="s">
         <v>180</v>
       </c>
@@ -4371,6 +4893,9 @@
       <c r="D176" t="s">
         <v>266</v>
       </c>
+      <c r="E176">
+        <v>6.4</v>
+      </c>
       <c r="F176" s="1" t="s">
         <v>181</v>
       </c>
@@ -4388,6 +4913,9 @@
       <c r="D177" t="s">
         <v>266</v>
       </c>
+      <c r="E177">
+        <v>6.4</v>
+      </c>
       <c r="F177" s="1" t="s">
         <v>182</v>
       </c>
@@ -4405,6 +4933,9 @@
       <c r="D178" t="s">
         <v>267</v>
       </c>
+      <c r="E178">
+        <v>6.4</v>
+      </c>
       <c r="F178" s="1" t="s">
         <v>183</v>
       </c>
@@ -4422,6 +4953,9 @@
       <c r="D179" t="s">
         <v>267</v>
       </c>
+      <c r="E179">
+        <v>6.4</v>
+      </c>
       <c r="F179" s="1" t="s">
         <v>184</v>
       </c>
@@ -4439,6 +4973,9 @@
       <c r="D180" t="s">
         <v>267</v>
       </c>
+      <c r="E180">
+        <v>6.4</v>
+      </c>
       <c r="F180" s="1" t="s">
         <v>185</v>
       </c>
@@ -4456,6 +4993,9 @@
       <c r="D181" t="s">
         <v>267</v>
       </c>
+      <c r="E181">
+        <v>6.4</v>
+      </c>
       <c r="F181" s="1" t="s">
         <v>186</v>
       </c>
@@ -4473,6 +5013,9 @@
       <c r="D182" t="s">
         <v>267</v>
       </c>
+      <c r="E182">
+        <v>6.4</v>
+      </c>
       <c r="F182" s="1" t="s">
         <v>187</v>
       </c>
@@ -4490,6 +5033,9 @@
       <c r="D183" t="s">
         <v>267</v>
       </c>
+      <c r="E183">
+        <v>6.4</v>
+      </c>
       <c r="F183" s="1" t="s">
         <v>188</v>
       </c>
@@ -4507,6 +5053,9 @@
       <c r="D184" t="s">
         <v>267</v>
       </c>
+      <c r="E184">
+        <v>6.4</v>
+      </c>
       <c r="F184" s="1" t="s">
         <v>189</v>
       </c>
@@ -4524,6 +5073,9 @@
       <c r="D185">
         <v>0</v>
       </c>
+      <c r="E185">
+        <v>7</v>
+      </c>
       <c r="F185" s="1" t="s">
         <v>190</v>
       </c>
@@ -4541,6 +5093,9 @@
       <c r="D186">
         <v>0</v>
       </c>
+      <c r="E186">
+        <v>7</v>
+      </c>
       <c r="F186" s="1" t="s">
         <v>191</v>
       </c>
@@ -4558,6 +5113,9 @@
       <c r="D187">
         <v>0</v>
       </c>
+      <c r="E187">
+        <v>7</v>
+      </c>
       <c r="F187" s="1" t="s">
         <v>192</v>
       </c>
@@ -4575,6 +5133,9 @@
       <c r="D188" t="s">
         <v>268</v>
       </c>
+      <c r="E188">
+        <v>6.4</v>
+      </c>
       <c r="F188" s="1" t="s">
         <v>193</v>
       </c>
@@ -4592,6 +5153,9 @@
       <c r="D189" t="s">
         <v>268</v>
       </c>
+      <c r="E189">
+        <v>6.4</v>
+      </c>
       <c r="F189" s="1" t="s">
         <v>194</v>
       </c>
@@ -4609,6 +5173,9 @@
       <c r="D190">
         <v>0</v>
       </c>
+      <c r="E190">
+        <v>7</v>
+      </c>
       <c r="F190" s="1" t="s">
         <v>195</v>
       </c>
@@ -4626,6 +5193,9 @@
       <c r="D191">
         <v>0</v>
       </c>
+      <c r="E191">
+        <v>7</v>
+      </c>
       <c r="F191" s="1" t="s">
         <v>196</v>
       </c>
@@ -4643,6 +5213,9 @@
       <c r="D192">
         <v>0</v>
       </c>
+      <c r="E192">
+        <v>7</v>
+      </c>
       <c r="F192" s="1" t="s">
         <v>197</v>
       </c>
@@ -4660,6 +5233,9 @@
       <c r="D193">
         <v>0</v>
       </c>
+      <c r="E193">
+        <v>7</v>
+      </c>
       <c r="F193" s="1" t="s">
         <v>198</v>
       </c>
@@ -4677,6 +5253,9 @@
       <c r="D194">
         <v>0</v>
       </c>
+      <c r="E194">
+        <v>7</v>
+      </c>
       <c r="F194" s="1" t="s">
         <v>199</v>
       </c>
@@ -4694,6 +5273,9 @@
       <c r="D195">
         <v>0</v>
       </c>
+      <c r="E195">
+        <v>7</v>
+      </c>
       <c r="F195" s="1" t="s">
         <v>200</v>
       </c>
@@ -4711,6 +5293,9 @@
       <c r="D196">
         <v>0</v>
       </c>
+      <c r="E196">
+        <v>7</v>
+      </c>
       <c r="F196" s="1" t="s">
         <v>201</v>
       </c>
@@ -4728,6 +5313,9 @@
       <c r="D197">
         <v>0</v>
       </c>
+      <c r="E197">
+        <v>7</v>
+      </c>
       <c r="F197" s="1" t="s">
         <v>202</v>
       </c>
@@ -4745,6 +5333,9 @@
       <c r="D198" t="s">
         <v>267</v>
       </c>
+      <c r="E198">
+        <v>3.5</v>
+      </c>
       <c r="F198" s="1" t="s">
         <v>203</v>
       </c>
@@ -4762,6 +5353,9 @@
       <c r="D199" t="s">
         <v>267</v>
       </c>
+      <c r="E199">
+        <v>3.5</v>
+      </c>
       <c r="F199" s="1" t="s">
         <v>204</v>
       </c>
@@ -4779,6 +5373,9 @@
       <c r="D200" t="s">
         <v>267</v>
       </c>
+      <c r="E200">
+        <v>3.5</v>
+      </c>
       <c r="F200" s="1" t="s">
         <v>205</v>
       </c>
@@ -4796,6 +5393,9 @@
       <c r="D201" t="s">
         <v>267</v>
       </c>
+      <c r="E201">
+        <v>3.5</v>
+      </c>
       <c r="F201" s="1" t="s">
         <v>206</v>
       </c>
@@ -4813,6 +5413,9 @@
       <c r="D202" t="s">
         <v>267</v>
       </c>
+      <c r="E202">
+        <v>6.4</v>
+      </c>
       <c r="F202" s="1" t="s">
         <v>207</v>
       </c>
@@ -4830,6 +5433,9 @@
       <c r="D203" t="s">
         <v>267</v>
       </c>
+      <c r="E203">
+        <v>6.4</v>
+      </c>
       <c r="F203" s="1" t="s">
         <v>208</v>
       </c>
@@ -4847,6 +5453,9 @@
       <c r="D204" t="s">
         <v>267</v>
       </c>
+      <c r="E204">
+        <v>6.4</v>
+      </c>
       <c r="F204" s="1" t="s">
         <v>209</v>
       </c>
@@ -4864,6 +5473,9 @@
       <c r="D205" t="s">
         <v>267</v>
       </c>
+      <c r="E205">
+        <v>6.4</v>
+      </c>
       <c r="F205" s="1" t="s">
         <v>210</v>
       </c>
@@ -4881,6 +5493,9 @@
       <c r="D206" t="s">
         <v>267</v>
       </c>
+      <c r="E206">
+        <v>11</v>
+      </c>
       <c r="F206" s="1" t="s">
         <v>211</v>
       </c>
@@ -4898,6 +5513,9 @@
       <c r="D207" t="s">
         <v>267</v>
       </c>
+      <c r="E207">
+        <v>11</v>
+      </c>
       <c r="F207" s="1" t="s">
         <v>212</v>
       </c>
@@ -4915,6 +5533,9 @@
       <c r="D208" t="s">
         <v>267</v>
       </c>
+      <c r="E208">
+        <v>11</v>
+      </c>
       <c r="F208" s="1" t="s">
         <v>213</v>
       </c>
@@ -4932,6 +5553,9 @@
       <c r="D209" t="s">
         <v>267</v>
       </c>
+      <c r="E209">
+        <v>11</v>
+      </c>
       <c r="F209" s="1" t="s">
         <v>214</v>
       </c>
@@ -4949,6 +5573,9 @@
       <c r="D210" t="s">
         <v>267</v>
       </c>
+      <c r="E210">
+        <v>11</v>
+      </c>
       <c r="F210" s="1" t="s">
         <v>215</v>
       </c>
@@ -4966,6 +5593,9 @@
       <c r="D211" t="s">
         <v>267</v>
       </c>
+      <c r="E211">
+        <v>11</v>
+      </c>
       <c r="F211" s="1" t="s">
         <v>216</v>
       </c>
@@ -4983,6 +5613,9 @@
       <c r="D212" t="s">
         <v>267</v>
       </c>
+      <c r="E212">
+        <v>11</v>
+      </c>
       <c r="F212" s="1" t="s">
         <v>217</v>
       </c>
@@ -5000,6 +5633,9 @@
       <c r="D213" t="s">
         <v>267</v>
       </c>
+      <c r="E213">
+        <v>11</v>
+      </c>
       <c r="F213" s="1" t="s">
         <v>218</v>
       </c>
@@ -5017,6 +5653,9 @@
       <c r="D214" t="s">
         <v>267</v>
       </c>
+      <c r="E214">
+        <v>11</v>
+      </c>
       <c r="F214" s="1" t="s">
         <v>219</v>
       </c>
@@ -5034,6 +5673,9 @@
       <c r="D215" t="s">
         <v>267</v>
       </c>
+      <c r="E215">
+        <v>11</v>
+      </c>
       <c r="F215" s="1" t="s">
         <v>220</v>
       </c>
@@ -5051,6 +5693,9 @@
       <c r="D216" t="s">
         <v>267</v>
       </c>
+      <c r="E216">
+        <v>11</v>
+      </c>
       <c r="F216" s="1" t="s">
         <v>221</v>
       </c>
@@ -5068,6 +5713,9 @@
       <c r="D217" t="s">
         <v>267</v>
       </c>
+      <c r="E217">
+        <v>11</v>
+      </c>
       <c r="F217" s="1" t="s">
         <v>222</v>
       </c>
@@ -5085,6 +5733,9 @@
       <c r="D218" t="s">
         <v>267</v>
       </c>
+      <c r="E218">
+        <v>11</v>
+      </c>
       <c r="F218" s="1" t="s">
         <v>223</v>
       </c>
@@ -5102,6 +5753,9 @@
       <c r="D219" t="s">
         <v>270</v>
       </c>
+      <c r="E219">
+        <v>6.4</v>
+      </c>
       <c r="F219" s="1" t="s">
         <v>224</v>
       </c>
@@ -5119,6 +5773,9 @@
       <c r="D220" t="s">
         <v>270</v>
       </c>
+      <c r="E220">
+        <v>6.4</v>
+      </c>
       <c r="F220" s="1" t="s">
         <v>225</v>
       </c>
@@ -5136,6 +5793,9 @@
       <c r="D221" t="s">
         <v>270</v>
       </c>
+      <c r="E221">
+        <v>6.4</v>
+      </c>
       <c r="F221" s="1" t="s">
         <v>226</v>
       </c>
@@ -5153,6 +5813,9 @@
       <c r="D222" t="s">
         <v>270</v>
       </c>
+      <c r="E222">
+        <v>6.4</v>
+      </c>
       <c r="F222" s="1" t="s">
         <v>227</v>
       </c>
@@ -5170,6 +5833,9 @@
       <c r="D223" t="s">
         <v>270</v>
       </c>
+      <c r="E223">
+        <v>6.4</v>
+      </c>
       <c r="F223" s="1" t="s">
         <v>228</v>
       </c>
@@ -5187,6 +5853,9 @@
       <c r="D224" t="s">
         <v>270</v>
       </c>
+      <c r="E224">
+        <v>6.4</v>
+      </c>
       <c r="F224" s="1" t="s">
         <v>229</v>
       </c>
@@ -5204,6 +5873,9 @@
       <c r="D225" t="s">
         <v>270</v>
       </c>
+      <c r="E225">
+        <v>6.4</v>
+      </c>
       <c r="F225" s="1" t="s">
         <v>230</v>
       </c>
@@ -5221,6 +5893,9 @@
       <c r="D226">
         <v>0</v>
       </c>
+      <c r="E226">
+        <v>7</v>
+      </c>
       <c r="F226" s="1" t="s">
         <v>231</v>
       </c>
@@ -5238,6 +5913,9 @@
       <c r="D227">
         <v>0</v>
       </c>
+      <c r="E227">
+        <v>7</v>
+      </c>
       <c r="F227" s="1" t="s">
         <v>232</v>
       </c>
@@ -5255,6 +5933,9 @@
       <c r="D228">
         <v>0</v>
       </c>
+      <c r="E228">
+        <v>7</v>
+      </c>
       <c r="F228" s="1" t="s">
         <v>233</v>
       </c>
@@ -5272,6 +5953,9 @@
       <c r="D229">
         <v>0</v>
       </c>
+      <c r="E229">
+        <v>7</v>
+      </c>
       <c r="F229" s="1" t="s">
         <v>234</v>
       </c>
@@ -5289,6 +5973,9 @@
       <c r="D230">
         <v>0</v>
       </c>
+      <c r="E230">
+        <v>7</v>
+      </c>
       <c r="F230" s="1" t="s">
         <v>235</v>
       </c>
@@ -5306,6 +5993,9 @@
       <c r="D231">
         <v>0</v>
       </c>
+      <c r="E231">
+        <v>7</v>
+      </c>
       <c r="F231" s="1" t="s">
         <v>236</v>
       </c>
@@ -5323,6 +6013,9 @@
       <c r="D232">
         <v>0</v>
       </c>
+      <c r="E232">
+        <v>7</v>
+      </c>
       <c r="F232" s="1" t="s">
         <v>237</v>
       </c>
@@ -5340,6 +6033,9 @@
       <c r="D233">
         <v>0</v>
       </c>
+      <c r="E233">
+        <v>7</v>
+      </c>
       <c r="F233" s="1" t="s">
         <v>238</v>
       </c>
@@ -5357,6 +6053,9 @@
       <c r="D234">
         <v>0</v>
       </c>
+      <c r="E234">
+        <v>7</v>
+      </c>
       <c r="F234" s="1" t="s">
         <v>239</v>
       </c>
@@ -5374,6 +6073,9 @@
       <c r="D235">
         <v>0</v>
       </c>
+      <c r="E235">
+        <v>7</v>
+      </c>
       <c r="F235" s="1" t="s">
         <v>240</v>
       </c>
@@ -5391,6 +6093,9 @@
       <c r="D236" t="s">
         <v>267</v>
       </c>
+      <c r="E236">
+        <v>6.4</v>
+      </c>
       <c r="F236" s="1" t="s">
         <v>241</v>
       </c>
@@ -5408,6 +6113,9 @@
       <c r="D237" t="s">
         <v>267</v>
       </c>
+      <c r="E237">
+        <v>6.4</v>
+      </c>
       <c r="F237" s="1" t="s">
         <v>242</v>
       </c>
@@ -5425,6 +6133,9 @@
       <c r="D238" t="s">
         <v>267</v>
       </c>
+      <c r="E238">
+        <v>6.4</v>
+      </c>
       <c r="F238" s="1" t="s">
         <v>243</v>
       </c>
@@ -5442,6 +6153,9 @@
       <c r="D239" t="s">
         <v>266</v>
       </c>
+      <c r="E239">
+        <v>3.5</v>
+      </c>
       <c r="F239" s="1" t="s">
         <v>244</v>
       </c>
@@ -5459,6 +6173,9 @@
       <c r="D240" t="s">
         <v>266</v>
       </c>
+      <c r="E240">
+        <v>3.5</v>
+      </c>
       <c r="F240" s="1" t="s">
         <v>245</v>
       </c>
@@ -5476,6 +6193,9 @@
       <c r="D241" t="s">
         <v>266</v>
       </c>
+      <c r="E241">
+        <v>3.5</v>
+      </c>
       <c r="F241" s="1" t="s">
         <v>246</v>
       </c>
@@ -5493,6 +6213,9 @@
       <c r="D242" t="s">
         <v>266</v>
       </c>
+      <c r="E242">
+        <v>3.5</v>
+      </c>
       <c r="F242" s="1" t="s">
         <v>247</v>
       </c>
@@ -5510,6 +6233,9 @@
       <c r="D243">
         <v>0</v>
       </c>
+      <c r="E243">
+        <v>7</v>
+      </c>
       <c r="F243" s="1" t="s">
         <v>248</v>
       </c>
@@ -5527,6 +6253,9 @@
       <c r="D244">
         <v>0</v>
       </c>
+      <c r="E244">
+        <v>7</v>
+      </c>
       <c r="F244" s="1" t="s">
         <v>249</v>
       </c>
@@ -5544,6 +6273,9 @@
       <c r="D245">
         <v>0</v>
       </c>
+      <c r="E245">
+        <v>7</v>
+      </c>
       <c r="F245" s="1" t="s">
         <v>250</v>
       </c>
@@ -5560,6 +6292,9 @@
       </c>
       <c r="D246">
         <v>0</v>
+      </c>
+      <c r="E246">
+        <v>7</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>251</v>

</xml_diff>